<commit_message>
Pressure NOR file changes
</commit_message>
<xml_diff>
--- a/nordson.omu/src/test/java/com/nordson/testData/NorfilePressure_Hydraulic_COD_LP_LV.xlsx
+++ b/nordson.omu/src/test/java/com/nordson/testData/NorfilePressure_Hydraulic_COD_LP_LV.xlsx
@@ -18,30 +18,30 @@
     <sheet name="Input_PSI_Runup" sheetId="263" r:id="rId9"/>
     <sheet name="Input_Runup_LineSpeedft_min" sheetId="274" r:id="rId10"/>
     <sheet name="Input_Runup_LineSpeedm_min" sheetId="273" r:id="rId11"/>
-    <sheet name="Output_Runup_Lnspeed_ftmin" r:id="rId33" sheetId="386"/>
-    <sheet name="Output_Runup_Lnspeed_mmin" r:id="rId46" sheetId="387"/>
-    <sheet name="Output_KPA_Manualadjust" r:id="rId34" sheetId="388"/>
-    <sheet name="Output_KPA_Mnladjst_ntv" r:id="rId35" sheetId="389"/>
-    <sheet name="Output_BAR_Manualadjust" r:id="rId36" sheetId="390"/>
-    <sheet name="Output_BAR_Mnladjst_ntv" r:id="rId37" sheetId="391"/>
-    <sheet name="Output_PSI_Manualadjust" r:id="rId38" sheetId="392"/>
-    <sheet name="Output_PSI_Mnladjst_ntv" r:id="rId39" sheetId="393"/>
-    <sheet name="Output_KPA_electronicadjust" r:id="rId40" sheetId="394"/>
-    <sheet name="Output_KPA_electronicadjust_Ntv" r:id="rId41" sheetId="395"/>
-    <sheet name="Output_BAR_electronicadjust" r:id="rId42" sheetId="396"/>
-    <sheet name="Output_BAR_electronicadjust_Ntv" r:id="rId43" sheetId="397"/>
-    <sheet name="Output_PSI_electronicadjust" r:id="rId44" sheetId="398"/>
-    <sheet name="Output_PSI_electronicadjust_Ntv" r:id="rId45" sheetId="399"/>
-    <sheet name="Output_KPA_Runup" r:id="rId47" sheetId="400"/>
-    <sheet name="Output_BAR_Runup" r:id="rId31" sheetId="401"/>
-    <sheet name="Output_PSI_Runup" r:id="rId32" sheetId="402"/>
+    <sheet name="Output_KPA_Manualadjust" r:id="rId34" sheetId="420"/>
+    <sheet name="Output_KPA_Mnladjst_ntv" r:id="rId35" sheetId="421"/>
+    <sheet name="Output_BAR_Manualadjust" r:id="rId36" sheetId="422"/>
+    <sheet name="Output_BAR_Mnladjst_ntv" r:id="rId37" sheetId="423"/>
+    <sheet name="Output_PSI_Manualadjust" r:id="rId38" sheetId="424"/>
+    <sheet name="Output_PSI_Mnladjst_ntv" r:id="rId39" sheetId="425"/>
+    <sheet name="Output_KPA_electronicadjust" r:id="rId40" sheetId="426"/>
+    <sheet name="Output_KPA_electronicadjust_Ntv" r:id="rId41" sheetId="427"/>
+    <sheet name="Output_BAR_electronicadjust" r:id="rId42" sheetId="428"/>
+    <sheet name="Output_BAR_electronicadjust_Ntv" r:id="rId43" sheetId="429"/>
+    <sheet name="Output_PSI_electronicadjust" r:id="rId44" sheetId="430"/>
+    <sheet name="Output_PSI_electronicadjust_Ntv" r:id="rId45" sheetId="431"/>
+    <sheet name="Output_KPA_Runup" r:id="rId47" sheetId="432"/>
+    <sheet name="Output_BAR_Runup" r:id="rId31" sheetId="433"/>
+    <sheet name="Output_PSI_Runup" r:id="rId32" sheetId="434"/>
+    <sheet name="Output_Runup_Lnspeed_ftmin" r:id="rId33" sheetId="435"/>
+    <sheet name="Output_Runup_Lnspeed_mmin" r:id="rId46" sheetId="436"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="117">
   <si>
     <t>Min_Pressure_KPA_UI</t>
   </si>
@@ -1563,532 +1563,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet386.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet387.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet388.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet389.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet390.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet391.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet392.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet393.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet394.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet395.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet396.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet397.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet398.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet399.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -2140,7 +1614,463 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet400.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet420.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet421.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet422.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet423.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet424.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet425.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet426.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet427.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet428.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet429.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet430.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet431.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet432.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2193,7 +2123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet401.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet433.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2246,7 +2176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet402.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet434.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2292,6 +2222,76 @@
       </c>
       <c r="F2" t="s">
         <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet435.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet436.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>